<commit_message>
DRB, SRB, TBeams, Slabs
</commit_message>
<xml_diff>
--- a/Design Calculators/Singly Reinforced Beams.xlsx
+++ b/Design Calculators/Singly Reinforced Beams.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Schoolwork\Excel Program\Design Calculators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5314FE7D-997F-44B8-8674-004A935A034D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED810A1B-97A5-45A5-85A5-A2CAB53490C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB4B3A85-F65C-4075-9FB4-543DD05A49C7}"/>
   </bookViews>
@@ -514,24 +514,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -542,9 +530,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -553,6 +538,21 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -628,7 +628,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55CB1AA9-CEDA-4ECB-887E-2AE3AB279B60}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -714,7 +714,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{599E9B31-37B0-4FBB-A286-7D549D4310CE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -800,7 +800,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BD06D7F-982F-4DE7-BB63-82701158B4C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -886,7 +886,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E25274-495B-455F-9D4E-50111FDD70FC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -972,7 +972,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EFAAD27-2358-4033-A5C6-FB1F2E2E93AE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1029,7 +1029,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD00E542-B2B7-44A8-B452-8DA89B6CD5EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1079,7 +1079,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{925C40C6-3E35-4F3A-9B3B-F9F9EECEEB68}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1432,7 +1432,7 @@
   <dimension ref="A2:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1461,10 +1461,10 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="24">
         <v>9000</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="24"/>
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -1474,11 +1474,11 @@
       <c r="G3" s="5">
         <v>28</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7">
+      <c r="L3" s="22"/>
+      <c r="M3" s="6">
         <v>23.6</v>
       </c>
       <c r="N3" t="s">
@@ -1489,10 +1489,10 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="24">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="24"/>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1502,11 +1502,11 @@
       <c r="G4" s="5">
         <v>420</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7">
+      <c r="L4" s="22"/>
+      <c r="M4" s="6">
         <v>200000</v>
       </c>
       <c r="N4" t="s">
@@ -1517,17 +1517,17 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="24">
         <v>32</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="24"/>
       <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f>IF((G3&gt;=17)*AND(G3&lt;=28),0.85,IF((G3&gt;28)*AND(G3&lt;55),ROUND((0.85-((0.05*(G3-28))/7)),2),IF((G3&gt;=55),0.65,0)))</f>
         <v>0.85</v>
       </c>
@@ -1535,10 +1535,10 @@
         <f>ROUND((0.85-((0.05*(G3-28))/7)),2)</f>
         <v>0.85</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="22"/>
       <c r="M5" s="5">
         <f>(M3*(I9*0.001)*(F9*0.001))</f>
         <v>7.080000000000001</v>
@@ -1551,39 +1551,39 @@
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="22"/>
       <c r="M6" s="5">
         <v>29.19</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="22"/>
       <c r="M7" s="5">
         <v>29.19</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <f>CEILING(C9,50)</f>
         <v>600</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="23" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1594,22 +1594,22 @@
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <f>ROUND(IF(A14=1,B3/16,IF(A14=2,B3/18.5,IF(A14=3,B3/21,IF(A14=4,B3/8,0)))),P14)</f>
         <v>562.5</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12">
+      <c r="E9" s="23"/>
+      <c r="F9" s="9">
         <v>750</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="12">
+      <c r="H9" s="23"/>
+      <c r="I9" s="9">
         <f>CEILING(F9/C6,50)</f>
         <v>400</v>
       </c>
@@ -1623,11 +1623,11 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="12">
+      <c r="L10" s="22"/>
+      <c r="M10" s="9">
         <f>(1.2*(M6+M5))+(1.6*(M7))</f>
         <v>90.228000000000009</v>
       </c>
@@ -1639,11 +1639,11 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="12">
+      <c r="F11" s="22"/>
+      <c r="G11" s="9">
         <f>40+B4+(B5/2)</f>
         <v>66</v>
       </c>
@@ -1660,22 +1660,22 @@
       <c r="F12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <f>F9-G11</f>
         <v>684</v>
       </c>
       <c r="H12" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="13">
+      <c r="L12" s="22"/>
+      <c r="M12" s="20">
         <f>ROUND(IF(A14=1,(M10*(B3^2)*0.000001)/8,IF(A14=2,B3/18.5,IF(A14=3,B3/21,IF(A14=4,B3/8,0)))),P14)</f>
         <v>913.55899999999997</v>
       </c>
-      <c r="N12" s="13"/>
+      <c r="N12" s="20"/>
       <c r="O12" t="s">
         <v>30</v>
       </c>
@@ -1689,7 +1689,7 @@
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="10" t="s">
         <v>32</v>
       </c>
       <c r="P14">
@@ -1697,86 +1697,86 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>0.9</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="20">
         <f>ROUND((M12*10^6)/(D16*I9*(G12^2)),P14)</f>
         <v>5.4240000000000004</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="H18" s="17" t="s">
+      <c r="E18" s="20"/>
+      <c r="H18" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I19" s="13">
+      <c r="I19" s="20">
         <f>ROUND(((0.25*SQRT(G3))/G4),K24)</f>
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="J19" s="13"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="20">
         <f>ROUND(((0.85*G3)/G4)*(1-SQRT(1-((2*D18)/(0.85*G3)))),K24)</f>
         <v>1.49E-2</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="I20" s="13">
+      <c r="E20" s="20"/>
+      <c r="I20" s="20">
         <f>ROUND((1.4/G4),K24)</f>
         <v>3.3E-3</v>
       </c>
-      <c r="J20" s="13"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L21" s="18" t="str">
+      <c r="L21" s="21" t="str">
         <f>IF((D20&gt;I22)*AND(D20&lt;D22),"STEEL YIELDS","STEEL DOES NOT YIELD")</f>
         <v>STEEL YIELDS</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
     </row>
     <row r="22" spans="1:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="20">
         <f>ROUND(((0.85*G3)/G4)*G5*(3/7),K24)</f>
         <v>2.06E-2</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="H22" s="17" t="s">
+      <c r="E22" s="20"/>
+      <c r="H22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="20">
         <f>MAX(I19,I20)</f>
         <v>3.3E-3</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
+      <c r="J22" s="20"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
     </row>
     <row r="23" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="10" t="s">
         <v>32</v>
       </c>
       <c r="K24">
@@ -1787,30 +1787,30 @@
       <c r="C25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="20">
         <f>ROUND(D20*I9*G12,P14)</f>
         <v>4076.64</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:14" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="20">
         <f>ROUND(((D25)/((3.14/4)*(B5^2))),P14)</f>
         <v>5.0709999999999997</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="G27" s="20">
+      <c r="E27" s="20"/>
+      <c r="G27" s="15">
         <f>ROUNDUP(D27,0)</f>
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1819,71 +1819,71 @@
       <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="20">
         <f>ROUND((I32*G4)/(0.85*G3*I9),P14)</f>
         <v>212.88900000000001</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="20"/>
       <c r="H32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="13">
+      <c r="I32" s="20">
         <f>ROUND(((PI()/4)*(B5^2)*(G27)),P14)</f>
         <v>4825.4859999999999</v>
       </c>
-      <c r="J32" s="13"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="20">
         <f>ROUND(D32/G5,P14)</f>
         <v>250.458</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="H34" s="21" t="s">
+      <c r="E34" s="20"/>
+      <c r="H34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="13">
+      <c r="I34" s="20">
         <f>ROUND((G4/M4),K24)</f>
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="J34" s="13"/>
+      <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L35" s="18" t="str">
+      <c r="L35" s="21" t="str">
         <f>IF(D36&gt;0.004,"STEEL YIELDS","STEEL DOES NOT YIELD")</f>
         <v>STEEL YIELDS</v>
       </c>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
     </row>
     <row r="36" spans="1:14" ht="16.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="20">
         <f>ROUND(((0.003*(G12-D34))/D34),K24)</f>
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="20"/>
       <c r="H36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I36" s="13">
+      <c r="I36" s="20">
         <f>IF(D36&lt;=I34,0.75,IF((D36&gt;I34)*AND(D36&lt;0.005),ROUND((0.75+0.15*((D36-I34)/(0.005-I34))),2),IF(D36&gt;=0.005,0.9,"ERROR")))</f>
         <v>0.9</v>
       </c>
-      <c r="J36" s="13"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
+      <c r="J36" s="20"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
     </row>
     <row r="37" spans="1:14" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1892,38 +1892,38 @@
       <c r="C41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="20">
         <f>ROUND((I36*I32*G4*(G12-(D32/2))*(1/10^6)),P14)</f>
         <v>1053.481</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="L41" s="18" t="str">
+      <c r="E41" s="20"/>
+      <c r="L41" s="21" t="str">
         <f>IF(D41&gt;M12,"SAFE","UNSAFE")</f>
         <v>SAFE</v>
       </c>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
     </row>
     <row r="42" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
     </row>
     <row r="43" spans="1:14" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="24">
+      <c r="E43" s="19">
         <f>G27</f>
         <v>6</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F43" s="19">
         <f>B5</f>
         <v>32</v>
       </c>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1964,11 +1964,24 @@
     </scenario>
   </scenarios>
   <mergeCells count="32">
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="L35:N36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="L41:N42"/>
     <mergeCell ref="L21:N22"/>
@@ -1978,24 +1991,11 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="L35:N36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="I36:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>